<commit_message>
added new raw data sheets & to mastersheet and modfied R script to make new figures
</commit_message>
<xml_diff>
--- a/data/2022-03-03_LakeErie_Mastersheet.xlsx
+++ b/data/2022-03-03_LakeErie_Mastersheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sklem\Documents\Etudes\Trent\Xenopoulos lab\Projects\Lake Erie &amp; animal excretion\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://trentu-my.sharepoint.com/personal/sandraklemet_trentu_ca/Documents/Documents/Etudes/Trent/Xenopoulos lab/Projects/LakeErie_animal-excretion/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA2E9A16-F367-47E5-9F32-F761EF32E94C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="79" documentId="13_ncr:1_{EA2E9A16-F367-47E5-9F32-F761EF32E94C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{11ECAE85-D764-4A2D-8D0F-766FE5F154D8}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="3" xr2:uid="{FCD5901F-55C5-46A6-83E9-A175C073FB2F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{FCD5901F-55C5-46A6-83E9-A175C073FB2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Fishing and Environmental data" sheetId="3" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1665" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1706" uniqueCount="149">
   <si>
     <t>Sampling run</t>
   </si>
@@ -459,6 +459,36 @@
   <si>
     <t>10/20/2021</t>
   </si>
+  <si>
+    <t>%C</t>
+  </si>
+  <si>
+    <t>%N</t>
+  </si>
+  <si>
+    <t>C:N</t>
+  </si>
+  <si>
+    <t>for fish, from stable isotopes analyses in Fisk lab; for mussels, from elementar analyses in Frost lab</t>
+  </si>
+  <si>
+    <t>from Xenopoulos lab</t>
+  </si>
+  <si>
+    <t>d13C</t>
+  </si>
+  <si>
+    <t>d15N</t>
+  </si>
+  <si>
+    <t>for fish, from stable isotopes analyses in Fisk lab - used data based on whole body or muscle analyses</t>
+  </si>
+  <si>
+    <t>%N tissue</t>
+  </si>
+  <si>
+    <t>%C tissue</t>
+  </si>
 </sst>
 </file>
 
@@ -505,7 +535,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -519,6 +549,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7113,15 +7146,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCB797C5-CB47-4805-AD51-BAF5F7220E5D}">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:AD17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="E7" workbookViewId="0">
+      <selection activeCell="AC21" sqref="AC21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -7165,7 +7198,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>84</v>
       </c>
@@ -7179,7 +7212,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>85</v>
       </c>
@@ -7187,7 +7220,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>86</v>
       </c>
@@ -7195,7 +7228,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>87</v>
       </c>
@@ -7203,44 +7236,156 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
       <c r="C12" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
         <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="M16" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="N16" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P16" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q16" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="R16" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="S16" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="T16" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="U16" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="V16" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="W16" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="X16" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="Y16" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="Z16" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA16" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="AB16" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="AC16" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="AD16" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="17" spans="25:30" x14ac:dyDescent="0.35">
+      <c r="Y17" t="s">
+        <v>142</v>
+      </c>
+      <c r="Z17" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>143</v>
+      </c>
+      <c r="AB17" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>146</v>
+      </c>
+      <c r="AD17" s="6" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -7251,13 +7396,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4782880F-19F5-4C97-B687-8149361B0730}">
-  <dimension ref="A1:Y160"/>
+  <dimension ref="A1:AD160"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E145" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="M126" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H146" sqref="H146"/>
+      <selection pane="bottomRight" activeCell="AD1" sqref="AD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7266,7 +7411,7 @@
     <col min="14" max="14" width="8.7265625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -7340,10 +7485,25 @@
         <v>100</v>
       </c>
       <c r="Y1" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="AA1" s="3" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB1" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>100</v>
       </c>
@@ -7423,11 +7583,11 @@
         <f>(W2/J2*60)/G2</f>
         <v>7238.4414137999984</v>
       </c>
-      <c r="Y2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>101</v>
       </c>
@@ -7507,11 +7667,11 @@
         <f t="shared" ref="X3:X46" si="6">(W3/J3*60)/G3</f>
         <v>3648.2018912250001</v>
       </c>
-      <c r="Y3" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA3" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>102</v>
       </c>
@@ -7591,11 +7751,11 @@
         <f t="shared" si="6"/>
         <v>3238.2886185290331</v>
       </c>
-      <c r="Y4" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA4" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>103</v>
       </c>
@@ -7675,11 +7835,11 @@
         <f t="shared" si="6"/>
         <v>3661.6451087177425</v>
       </c>
-      <c r="Y5" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA5" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>104</v>
       </c>
@@ -7759,11 +7919,11 @@
         <f t="shared" si="6"/>
         <v>4819.0041642919359</v>
       </c>
-      <c r="Y6" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA6" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>105</v>
       </c>
@@ -7843,11 +8003,11 @@
         <f t="shared" si="6"/>
         <v>3935.7271456199996</v>
       </c>
-      <c r="Y7" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA7" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>107</v>
       </c>
@@ -7927,11 +8087,11 @@
         <f t="shared" si="6"/>
         <v>3424.9940921045454</v>
       </c>
-      <c r="Y8" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA8" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>108</v>
       </c>
@@ -8011,11 +8171,11 @@
         <f t="shared" si="6"/>
         <v>2972.8641739499994</v>
       </c>
-      <c r="Y9" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA9" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>109</v>
       </c>
@@ -8095,11 +8255,11 @@
         <f t="shared" si="6"/>
         <v>14048.38427682857</v>
       </c>
-      <c r="Y10" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA10" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>110</v>
       </c>
@@ -8179,11 +8339,11 @@
         <f t="shared" si="6"/>
         <v>4287.1311989549995</v>
       </c>
-      <c r="Y11" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA11" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>111</v>
       </c>
@@ -8263,11 +8423,11 @@
         <f t="shared" si="6"/>
         <v>1129.06789665</v>
       </c>
-      <c r="Y12" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA12" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>112</v>
       </c>
@@ -8347,11 +8507,11 @@
         <f t="shared" si="6"/>
         <v>4114.6215824999999</v>
       </c>
-      <c r="Y13" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA13" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>113</v>
       </c>
@@ -8431,11 +8591,11 @@
         <f t="shared" si="6"/>
         <v>1532.2265103449995</v>
       </c>
-      <c r="Y14" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA14" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>114</v>
       </c>
@@ -8515,11 +8675,11 @@
         <f t="shared" si="6"/>
         <v>2363.0012786100006</v>
       </c>
-      <c r="Y15" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA15" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>115</v>
       </c>
@@ -8599,11 +8759,11 @@
         <f t="shared" si="6"/>
         <v>1193.7261317400003</v>
       </c>
-      <c r="Y16" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA16" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>116</v>
       </c>
@@ -8683,11 +8843,11 @@
         <f t="shared" si="6"/>
         <v>5928.3527493149995</v>
       </c>
-      <c r="Y17" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA17" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>117</v>
       </c>
@@ -8767,11 +8927,11 @@
         <f t="shared" si="6"/>
         <v>2118.7383727650003</v>
       </c>
-      <c r="Y18" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA18" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>118</v>
       </c>
@@ -8851,11 +9011,11 @@
         <f t="shared" si="6"/>
         <v>1649.0505306299999</v>
       </c>
-      <c r="Y19" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA19" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>119</v>
       </c>
@@ -8935,11 +9095,11 @@
         <f t="shared" si="6"/>
         <v>2474.8802323800001</v>
       </c>
-      <c r="Y20" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA20" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>120</v>
       </c>
@@ -9019,11 +9179,11 @@
         <f t="shared" si="6"/>
         <v>8454.3676238549997</v>
       </c>
-      <c r="Y21" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA21" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>121</v>
       </c>
@@ -9103,11 +9263,11 @@
         <f t="shared" si="6"/>
         <v>2007.7299107699998</v>
       </c>
-      <c r="Y22" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA22" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>122</v>
       </c>
@@ -9187,11 +9347,11 @@
         <f t="shared" si="6"/>
         <v>4647.4761862199994</v>
       </c>
-      <c r="Y23" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA23" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>123</v>
       </c>
@@ -9267,11 +9427,11 @@
       <c r="X24" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="Y24" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA24" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>124</v>
       </c>
@@ -9347,11 +9507,11 @@
       <c r="X25" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="Y25" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA25" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>125</v>
       </c>
@@ -9431,11 +9591,11 @@
         <f t="shared" si="6"/>
         <v>2897.8977017538464</v>
       </c>
-      <c r="Y26" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA26" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>126</v>
       </c>
@@ -9516,11 +9676,11 @@
         <f t="shared" si="6"/>
         <v>24.669084985147059</v>
       </c>
-      <c r="Y27">
+      <c r="AA27">
         <v>1.3334962267205783</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>127</v>
       </c>
@@ -9600,11 +9760,11 @@
         <f t="shared" si="6"/>
         <v>16.318005637752812</v>
       </c>
-      <c r="Y28">
+      <c r="AA28">
         <v>1.3731681167778587</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>128</v>
       </c>
@@ -9684,11 +9844,11 @@
         <f t="shared" si="6"/>
         <v>4.2867681468750005</v>
       </c>
-      <c r="Y29">
+      <c r="AA29">
         <v>1.2970090764968623</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>129</v>
       </c>
@@ -9764,11 +9924,11 @@
       <c r="X30" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="Y30" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA30" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>130</v>
       </c>
@@ -9848,11 +10008,11 @@
         <f t="shared" si="6"/>
         <v>1006.0928500500004</v>
       </c>
-      <c r="Y31" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA31" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>131</v>
       </c>
@@ -9928,11 +10088,11 @@
       <c r="X32" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="Y32" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA32" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>132</v>
       </c>
@@ -10012,11 +10172,11 @@
         <f t="shared" si="6"/>
         <v>13165.302023427272</v>
       </c>
-      <c r="Y33" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA33" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>133</v>
       </c>
@@ -10096,11 +10256,11 @@
         <f t="shared" si="6"/>
         <v>8990.1693375272735</v>
       </c>
-      <c r="Y34" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA34" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>134</v>
       </c>
@@ -10180,11 +10340,11 @@
         <f t="shared" si="6"/>
         <v>7144.2401343900019</v>
       </c>
-      <c r="Y35" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA35" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>135</v>
       </c>
@@ -10264,11 +10424,11 @@
         <f t="shared" si="6"/>
         <v>11719.623423202942</v>
       </c>
-      <c r="Y36" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA36" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>136</v>
       </c>
@@ -10348,11 +10508,11 @@
         <f t="shared" si="6"/>
         <v>6357.1682467227274</v>
       </c>
-      <c r="Y37" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA37" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>137</v>
       </c>
@@ -10432,11 +10592,11 @@
         <f t="shared" si="6"/>
         <v>8009.2471858593763</v>
       </c>
-      <c r="Y38" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA38" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>138</v>
       </c>
@@ -10516,11 +10676,11 @@
         <f t="shared" si="6"/>
         <v>13443.876453735</v>
       </c>
-      <c r="Y39" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA39" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="40" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>139</v>
       </c>
@@ -10600,11 +10760,11 @@
         <f t="shared" si="6"/>
         <v>3154.3510400024998</v>
       </c>
-      <c r="Y40" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA40" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>140</v>
       </c>
@@ -10684,11 +10844,11 @@
         <f t="shared" si="6"/>
         <v>653.24491680483857</v>
       </c>
-      <c r="Y41" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA41" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="42" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>141</v>
       </c>
@@ -10769,11 +10929,11 @@
         <f t="shared" si="6"/>
         <v>-5.7080499533898319</v>
       </c>
-      <c r="Y42" s="6">
+      <c r="AA42" s="6">
         <v>1.422656205454786</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>142</v>
       </c>
@@ -10849,11 +11009,11 @@
       <c r="X43" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="Y43" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA43" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="44" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>143</v>
       </c>
@@ -10934,11 +11094,11 @@
         <f t="shared" si="6"/>
         <v>4.1221994636363624</v>
       </c>
-      <c r="Y44">
+      <c r="AA44">
         <v>1.1525255462158601</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>144</v>
       </c>
@@ -11019,11 +11179,11 @@
         <f t="shared" si="6"/>
         <v>33.487499690217398</v>
       </c>
-      <c r="Y45">
+      <c r="AA45">
         <v>1.4162833266498689</v>
       </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>145</v>
       </c>
@@ -11104,11 +11264,11 @@
         <f t="shared" si="6"/>
         <v>6.4780855722222181</v>
       </c>
-      <c r="Y46">
+      <c r="AA46">
         <v>1.0982607475444324</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>146</v>
       </c>
@@ -11184,11 +11344,11 @@
       <c r="X47" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="Y47" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA47" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="48" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A48" s="6">
         <v>200</v>
       </c>
@@ -11258,11 +11418,26 @@
         <f t="shared" si="4"/>
         <v>41.571333658536588</v>
       </c>
-      <c r="Y48" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y48" s="8">
+        <v>41.268769832931916</v>
+      </c>
+      <c r="Z48" s="8">
+        <v>11.657486598331682</v>
+      </c>
+      <c r="AA48" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB48">
+        <v>3.5401087090966885</v>
+      </c>
+      <c r="AC48" s="8">
+        <v>-19.862049406277322</v>
+      </c>
+      <c r="AD48" s="8">
+        <v>8.3847586859687198</v>
+      </c>
+    </row>
+    <row r="49" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A49" s="6">
         <v>201</v>
       </c>
@@ -11332,11 +11507,26 @@
         <f t="shared" si="4"/>
         <v>57.719015121951223</v>
       </c>
-      <c r="Y49" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y49" s="8">
+        <v>48.023862040266181</v>
+      </c>
+      <c r="Z49" s="8">
+        <v>13.571514530090662</v>
+      </c>
+      <c r="AA49" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB49">
+        <v>3.5385779482303192</v>
+      </c>
+      <c r="AC49" s="8">
+        <v>-18.679240911920768</v>
+      </c>
+      <c r="AD49" s="8">
+        <v>8.7270334952932984</v>
+      </c>
+    </row>
+    <row r="50" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A50" s="6">
         <v>202</v>
       </c>
@@ -11406,11 +11596,26 @@
         <f t="shared" si="4"/>
         <v>38.309009268292691</v>
       </c>
-      <c r="Y50" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y50" s="8">
+        <v>50.463596319797603</v>
+      </c>
+      <c r="Z50" s="8">
+        <v>13.483840144439847</v>
+      </c>
+      <c r="AA50" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB50">
+        <v>3.7425240717205184</v>
+      </c>
+      <c r="AC50" s="8">
+        <v>-20.053856189145954</v>
+      </c>
+      <c r="AD50" s="8">
+        <v>9.1981531322659187</v>
+      </c>
+    </row>
+    <row r="51" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A51" s="6">
         <v>203</v>
       </c>
@@ -11480,11 +11685,26 @@
         <f t="shared" si="4"/>
         <v>77.084064878048778</v>
       </c>
-      <c r="Y51" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y51" s="8">
+        <v>44.829084275094807</v>
+      </c>
+      <c r="Z51" s="8">
+        <v>13.217583694498243</v>
+      </c>
+      <c r="AA51" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB51">
+        <v>3.3916247713078378</v>
+      </c>
+      <c r="AC51" s="8">
+        <v>-17.393536070504485</v>
+      </c>
+      <c r="AD51" s="8">
+        <v>7.8831490516137386</v>
+      </c>
+    </row>
+    <row r="52" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A52" s="6">
         <v>204</v>
       </c>
@@ -11554,11 +11774,26 @@
         <f t="shared" si="4"/>
         <v>39.334311219512195</v>
       </c>
-      <c r="Y52" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y52" s="8">
+        <v>48.105372156855218</v>
+      </c>
+      <c r="Z52" s="8">
+        <v>11.913260402967483</v>
+      </c>
+      <c r="AA52" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB52">
+        <v>4.0379686609446237</v>
+      </c>
+      <c r="AC52" s="8">
+        <v>-19.45645798000303</v>
+      </c>
+      <c r="AD52" s="8">
+        <v>7.8546261508366904</v>
+      </c>
+    </row>
+    <row r="53" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A53" s="6">
         <v>205</v>
       </c>
@@ -11627,11 +11862,26 @@
         <f t="shared" si="4"/>
         <v>86.574244499999992</v>
       </c>
-      <c r="Y53" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y53" s="8">
+        <v>47.845184510930856</v>
+      </c>
+      <c r="Z53" s="8">
+        <v>13.707852722485121</v>
+      </c>
+      <c r="AA53" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB53">
+        <v>3.4903485964982646</v>
+      </c>
+      <c r="AC53" s="8">
+        <v>-20.02688336030505</v>
+      </c>
+      <c r="AD53" s="8">
+        <v>7.8438071195074652</v>
+      </c>
+    </row>
+    <row r="54" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A54" s="6">
         <v>206</v>
       </c>
@@ -11700,11 +11950,26 @@
         <f t="shared" si="4"/>
         <v>22.593634054054053</v>
       </c>
-      <c r="Y54" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y54" s="8">
+        <v>48.77149830380344</v>
+      </c>
+      <c r="Z54" s="8">
+        <v>14.145544654748724</v>
+      </c>
+      <c r="AA54" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB54">
+        <v>3.4478346005171758</v>
+      </c>
+      <c r="AC54" s="8">
+        <v>-19.302612956243816</v>
+      </c>
+      <c r="AD54" s="8">
+        <v>9.9633537117329318</v>
+      </c>
+    </row>
+    <row r="55" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A55" s="6">
         <v>207</v>
       </c>
@@ -11774,11 +12039,26 @@
         <f t="shared" si="4"/>
         <v>46.960545789473677</v>
       </c>
-      <c r="Y55" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y55" s="8">
+        <v>45.101389328059625</v>
+      </c>
+      <c r="Z55" s="8">
+        <v>13.727274392063153</v>
+      </c>
+      <c r="AA55" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB55">
+        <v>3.2855312744485086</v>
+      </c>
+      <c r="AC55" s="8">
+        <v>-16.767167045199113</v>
+      </c>
+      <c r="AD55" s="8">
+        <v>7.7965968009799376</v>
+      </c>
+    </row>
+    <row r="56" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A56" s="6">
         <v>208</v>
       </c>
@@ -11848,11 +12128,26 @@
         <f t="shared" si="4"/>
         <v>22.662043783783776</v>
       </c>
-      <c r="Y56" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y56" s="8">
+        <v>40.054321441921495</v>
+      </c>
+      <c r="Z56" s="8">
+        <v>11.864405784167309</v>
+      </c>
+      <c r="AA56" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB56">
+        <v>3.3760073762288862</v>
+      </c>
+      <c r="AC56" s="8">
+        <v>-17.117813820130827</v>
+      </c>
+      <c r="AD56" s="8">
+        <v>8.0729738740265073</v>
+      </c>
+    </row>
+    <row r="57" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A57" s="6">
         <v>209</v>
       </c>
@@ -11922,11 +12217,26 @@
         <f t="shared" si="4"/>
         <v>46.007379473684203</v>
       </c>
-      <c r="Y57" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y57" s="8">
+        <v>46.622035665190204</v>
+      </c>
+      <c r="Z57" s="8">
+        <v>13.9946723121618</v>
+      </c>
+      <c r="AA57" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB57">
+        <v>3.3314131710446855</v>
+      </c>
+      <c r="AC57" s="8">
+        <v>-18.102821569654104</v>
+      </c>
+      <c r="AD57" s="8">
+        <v>8.5932709261319697</v>
+      </c>
+    </row>
+    <row r="58" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A58" s="6">
         <v>210</v>
       </c>
@@ -11996,11 +12306,26 @@
         <f t="shared" si="4"/>
         <v>25.335412105263153</v>
       </c>
-      <c r="Y58" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y58" s="8">
+        <v>45.399814637054185</v>
+      </c>
+      <c r="Z58" s="8">
+        <v>12.493075857076738</v>
+      </c>
+      <c r="AA58" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB58">
+        <v>3.6339981567739645</v>
+      </c>
+      <c r="AC58" s="8">
+        <v>-20.224684105138326</v>
+      </c>
+      <c r="AD58" s="8">
+        <v>10.514140761220755</v>
+      </c>
+    </row>
+    <row r="59" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A59" s="6">
         <v>211</v>
       </c>
@@ -12069,11 +12394,26 @@
         <f t="shared" si="4"/>
         <v>33.277186153846159</v>
       </c>
-      <c r="Y59" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y59" s="8">
+        <v>46.441976239614213</v>
+      </c>
+      <c r="Z59" s="8">
+        <v>13.763615704001237</v>
+      </c>
+      <c r="AA59" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB59">
+        <v>3.3742569713068211</v>
+      </c>
+      <c r="AC59" s="8">
+        <v>-17.008923511106449</v>
+      </c>
+      <c r="AD59" s="8">
+        <v>8.3454167538624482</v>
+      </c>
+    </row>
+    <row r="60" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A60" s="6">
         <v>212</v>
       </c>
@@ -12142,11 +12482,26 @@
         <f t="shared" si="4"/>
         <v>30.614826857142855</v>
       </c>
-      <c r="Y60" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y60" s="8">
+        <v>45.506955377509499</v>
+      </c>
+      <c r="Z60" s="8">
+        <v>12.921571127034527</v>
+      </c>
+      <c r="AA60" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB60">
+        <v>3.5217819048567391</v>
+      </c>
+      <c r="AC60" s="8">
+        <v>-19.060856490336484</v>
+      </c>
+      <c r="AD60" s="8">
+        <v>7.365802644416247</v>
+      </c>
+    </row>
+    <row r="61" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A61" s="6">
         <v>213</v>
       </c>
@@ -12215,11 +12570,26 @@
         <f t="shared" si="4"/>
         <v>44.228556000000005</v>
       </c>
-      <c r="Y61" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y61">
+        <v>43.226796733858045</v>
+      </c>
+      <c r="Z61">
+        <v>12.927991861589712</v>
+      </c>
+      <c r="AA61" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB61">
+        <v>3.344076243367573</v>
+      </c>
+      <c r="AC61">
+        <v>-17.951307531103364</v>
+      </c>
+      <c r="AD61">
+        <v>8.2818139636239732</v>
+      </c>
+    </row>
+    <row r="62" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A62" s="6">
         <v>214</v>
       </c>
@@ -12288,11 +12658,26 @@
         <f t="shared" si="4"/>
         <v>94.284109999999998</v>
       </c>
-      <c r="Y62" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y62">
+        <v>45.855573752930248</v>
+      </c>
+      <c r="Z62">
+        <v>13.107901323778782</v>
+      </c>
+      <c r="AA62" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB62">
+        <v>3.4983154526609512</v>
+      </c>
+      <c r="AC62">
+        <v>-15.374569882079996</v>
+      </c>
+      <c r="AD62">
+        <v>7.7415180960311538</v>
+      </c>
+    </row>
+    <row r="63" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A63" s="6">
         <v>215</v>
       </c>
@@ -12361,11 +12746,26 @@
         <f t="shared" si="4"/>
         <v>34.708825945945939</v>
       </c>
-      <c r="Y63" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y63">
+        <v>45.151981351258598</v>
+      </c>
+      <c r="Z63">
+        <v>12.851598659115895</v>
+      </c>
+      <c r="AA63" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB63">
+        <v>3.5133357762640212</v>
+      </c>
+      <c r="AC63">
+        <v>-20.312595547286449</v>
+      </c>
+      <c r="AD63">
+        <v>9.8787685577044435</v>
+      </c>
+    </row>
+    <row r="64" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A64" s="6">
         <v>216</v>
       </c>
@@ -12434,11 +12834,26 @@
         <f t="shared" si="4"/>
         <v>34.881903243243237</v>
       </c>
-      <c r="Y64" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y64">
+        <v>48.493961232660318</v>
+      </c>
+      <c r="Z64">
+        <v>13.551373480254691</v>
+      </c>
+      <c r="AA64" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB64">
+        <v>3.5785273945345426</v>
+      </c>
+      <c r="AC64">
+        <v>-16.501434731433196</v>
+      </c>
+      <c r="AD64">
+        <v>8.9266938007326342</v>
+      </c>
+    </row>
+    <row r="65" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A65" s="6">
         <v>217</v>
       </c>
@@ -12507,11 +12922,26 @@
         <f t="shared" si="4"/>
         <v>77.644572631578967</v>
       </c>
-      <c r="Y65" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y65">
+        <v>46.919444510957248</v>
+      </c>
+      <c r="Z65">
+        <v>11.960143176782946</v>
+      </c>
+      <c r="AA65" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB65">
+        <v>3.9229835142807796</v>
+      </c>
+      <c r="AC65">
+        <v>-19.761151046539133</v>
+      </c>
+      <c r="AD65">
+        <v>8.0562535528813406</v>
+      </c>
+    </row>
+    <row r="66" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A66" s="6">
         <v>218</v>
       </c>
@@ -12580,11 +13010,26 @@
         <f t="shared" si="4"/>
         <v>12.585798947368419</v>
       </c>
-      <c r="Y66" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y66">
+        <v>41.291728835214329</v>
+      </c>
+      <c r="Z66">
+        <v>11.071236139224085</v>
+      </c>
+      <c r="AA66" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB66">
+        <v>3.7296403324758467</v>
+      </c>
+      <c r="AC66">
+        <v>-17.658269390609625</v>
+      </c>
+      <c r="AD66">
+        <v>7.7621726103869495</v>
+      </c>
+    </row>
+    <row r="67" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A67" s="6">
         <v>219</v>
       </c>
@@ -12650,11 +13095,26 @@
         <f t="shared" ref="U67:U130" si="19">(T67/J67*60)/G67</f>
         <v>8080.9046181818194</v>
       </c>
-      <c r="Y67" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y67">
+        <v>48.925217850405573</v>
+      </c>
+      <c r="Z67">
+        <v>14.556161387128618</v>
+      </c>
+      <c r="AA67" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB67">
+        <v>3.3611346116063276</v>
+      </c>
+      <c r="AC67" s="8">
+        <v>-16.16477386775232</v>
+      </c>
+      <c r="AD67" s="8">
+        <v>7.7366003545178721</v>
+      </c>
+    </row>
+    <row r="68" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A68" s="6">
         <v>220</v>
       </c>
@@ -12720,11 +13180,26 @@
         <f t="shared" si="19"/>
         <v>4382.5390645161297</v>
       </c>
-      <c r="Y68" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y68">
+        <v>47.215207275148913</v>
+      </c>
+      <c r="Z68">
+        <v>13.937784692137903</v>
+      </c>
+      <c r="AA68" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB68">
+        <v>3.3875689945032876</v>
+      </c>
+      <c r="AC68" s="8">
+        <v>-17.541387132299054</v>
+      </c>
+      <c r="AD68" s="8">
+        <v>9.6033750329605319</v>
+      </c>
+    </row>
+    <row r="69" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A69" s="6">
         <v>221</v>
       </c>
@@ -12790,11 +13265,11 @@
         <f t="shared" si="19"/>
         <v>2158.6055526315786</v>
       </c>
-      <c r="Y69" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA69" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="70" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A70" s="6">
         <v>222</v>
       </c>
@@ -12860,11 +13335,11 @@
         <f t="shared" si="19"/>
         <v>2138.7438947368414</v>
       </c>
-      <c r="Y70" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA70" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="71" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A71" s="6">
         <v>223</v>
       </c>
@@ -12930,11 +13405,11 @@
         <f t="shared" si="19"/>
         <v>2978.0781081081082</v>
       </c>
-      <c r="Y71" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA71" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="72" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A72" s="6">
         <v>224</v>
       </c>
@@ -13000,11 +13475,11 @@
         <f t="shared" si="19"/>
         <v>2019.3329999999999</v>
       </c>
-      <c r="Y72" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA72" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="73" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A73" s="6">
         <v>225</v>
       </c>
@@ -13070,11 +13545,11 @@
         <f t="shared" si="19"/>
         <v>2096.6512058823528</v>
       </c>
-      <c r="Y73" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA73" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="74" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A74" s="6">
         <v>226</v>
       </c>
@@ -13140,11 +13615,11 @@
         <f t="shared" si="19"/>
         <v>3738.0372580645153</v>
       </c>
-      <c r="Y74" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA74" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="75" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A75" s="6">
         <v>227</v>
       </c>
@@ -13210,11 +13685,11 @@
         <f t="shared" si="19"/>
         <v>1339.1853000000003</v>
       </c>
-      <c r="Y75" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA75" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="76" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A76" s="6">
         <v>228</v>
       </c>
@@ -13280,11 +13755,11 @@
         <f t="shared" si="19"/>
         <v>1975.0182413793104</v>
       </c>
-      <c r="Y76" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA76" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="77" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A77" s="6">
         <v>229</v>
       </c>
@@ -13351,11 +13826,11 @@
         <f t="shared" si="19"/>
         <v>3364.1324444444449</v>
       </c>
-      <c r="Y77" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA77" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="78" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A78" s="6">
         <v>230</v>
       </c>
@@ -13422,11 +13897,11 @@
         <f t="shared" si="19"/>
         <v>2090.6504571428577</v>
       </c>
-      <c r="Y78" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA78" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="79" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A79" s="6">
         <v>231</v>
       </c>
@@ -13493,11 +13968,26 @@
         <f t="shared" si="19"/>
         <v>1550.6940454545452</v>
       </c>
-      <c r="Y79" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y79" s="8">
+        <v>52.430476865432681</v>
+      </c>
+      <c r="Z79" s="8">
+        <v>16.328197300791</v>
+      </c>
+      <c r="AA79" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB79" s="8">
+        <v>3.2110389101491776</v>
+      </c>
+      <c r="AC79" s="8">
+        <v>-16.232705436684963</v>
+      </c>
+      <c r="AD79" s="8">
+        <v>11.011816202365111</v>
+      </c>
+    </row>
+    <row r="80" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A80" s="6">
         <v>232</v>
       </c>
@@ -13564,11 +14054,11 @@
         <f t="shared" si="19"/>
         <v>716.06372727272731</v>
       </c>
-      <c r="Y80" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="81" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA80" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="81" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A81" s="6">
         <v>233</v>
       </c>
@@ -13633,11 +14123,11 @@
         <f t="shared" si="19"/>
         <v>858.15004545454565</v>
       </c>
-      <c r="Y81" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA81" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="82" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A82" s="6">
         <v>234</v>
       </c>
@@ -13704,11 +14194,11 @@
         <f t="shared" si="19"/>
         <v>1350.490640625</v>
       </c>
-      <c r="Y82" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="83" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA82" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="83" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A83" s="6">
         <v>235</v>
       </c>
@@ -13775,11 +14265,11 @@
         <f t="shared" si="19"/>
         <v>1197.4402031249999</v>
       </c>
-      <c r="Y83" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="84" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA83" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="84" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A84" s="6">
         <v>236</v>
       </c>
@@ -13845,11 +14335,11 @@
         <f t="shared" si="19"/>
         <v>719.38295454545448</v>
       </c>
-      <c r="Y84" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="85" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA84" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="85" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A85" s="6">
         <v>237</v>
       </c>
@@ -13915,11 +14405,11 @@
         <f t="shared" si="19"/>
         <v>1028.9478281250001</v>
       </c>
-      <c r="Y85" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="86" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA85" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="86" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A86" s="6">
         <v>238</v>
       </c>
@@ -13985,11 +14475,11 @@
         <f t="shared" si="19"/>
         <v>812.27308235294117</v>
       </c>
-      <c r="Y86" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="87" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA86" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="87" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A87" s="6">
         <v>239</v>
       </c>
@@ -14055,11 +14545,11 @@
         <f t="shared" si="19"/>
         <v>125.50002181818181</v>
       </c>
-      <c r="Y87" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="88" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA87" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="88" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A88" s="6">
         <v>240</v>
       </c>
@@ -14125,11 +14615,11 @@
         <f t="shared" si="19"/>
         <v>201.96794909090912</v>
       </c>
-      <c r="Y88" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="89" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA88" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="89" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A89" s="6">
         <v>241</v>
       </c>
@@ -14195,11 +14685,11 @@
         <f t="shared" si="19"/>
         <v>274.53256000000005</v>
       </c>
-      <c r="Y89" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="90" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA89" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="90" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A90" s="6">
         <v>242</v>
       </c>
@@ -14265,11 +14755,11 @@
         <f t="shared" si="19"/>
         <v>476.4371999999999</v>
       </c>
-      <c r="Y90" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="91" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA90" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="91" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A91" s="6">
         <v>243</v>
       </c>
@@ -14335,11 +14825,11 @@
         <f t="shared" si="19"/>
         <v>576.11345806451618</v>
       </c>
-      <c r="Y91" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="92" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA91" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="92" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A92" s="6">
         <v>244</v>
       </c>
@@ -14405,11 +14895,11 @@
         <f t="shared" si="19"/>
         <v>303.0658499999999</v>
       </c>
-      <c r="Y92" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="93" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA92" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="93" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A93" s="6">
         <v>245</v>
       </c>
@@ -14472,11 +14962,11 @@
       <c r="U93" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="Y93" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="94" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA93" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="94" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A94" s="6">
         <v>246</v>
       </c>
@@ -14541,11 +15031,11 @@
         <f t="shared" si="19"/>
         <v>3.3051502702702726</v>
       </c>
-      <c r="Y94" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="95" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA94" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="95" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A95" s="6">
         <v>247</v>
       </c>
@@ -14612,11 +15102,11 @@
         <f t="shared" si="19"/>
         <v>3424.9003076923082</v>
       </c>
-      <c r="Y95" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="96" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA95" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="96" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A96" s="6">
         <v>248</v>
       </c>
@@ -14682,11 +15172,11 @@
         <f t="shared" si="19"/>
         <v>3357.9206846153843</v>
       </c>
-      <c r="Y96" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="97" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA96" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="97" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A97" s="6">
         <v>249</v>
       </c>
@@ -14754,11 +15244,11 @@
         <f t="shared" si="19"/>
         <v>205.60192975609758</v>
       </c>
-      <c r="Y97" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="98" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA97" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="98" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A98" s="6">
         <v>250</v>
       </c>
@@ -14828,11 +15318,26 @@
         <f t="shared" si="19"/>
         <v>109.79866800000003</v>
       </c>
-      <c r="Y98" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="99" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y98">
+        <v>45.194361632360113</v>
+      </c>
+      <c r="Z98">
+        <v>13.320934387087064</v>
+      </c>
+      <c r="AA98" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB98">
+        <v>3.3927320951426836</v>
+      </c>
+      <c r="AC98">
+        <v>-18.502419033963751</v>
+      </c>
+      <c r="AD98">
+        <v>8.3955777172979467</v>
+      </c>
+    </row>
+    <row r="99" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A99" s="6">
         <v>251</v>
       </c>
@@ -14901,11 +15406,26 @@
         <f t="shared" si="19"/>
         <v>178.48648799999998</v>
       </c>
-      <c r="Y99" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="100" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y99">
+        <v>45.480914068686779</v>
+      </c>
+      <c r="Z99">
+        <v>13.760689982030001</v>
+      </c>
+      <c r="AA99" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB99">
+        <v>3.3051332548062646</v>
+      </c>
+      <c r="AC99">
+        <v>-18.245677663144804</v>
+      </c>
+      <c r="AD99">
+        <v>8.1132993544354353</v>
+      </c>
+    </row>
+    <row r="100" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A100" s="6">
         <v>252</v>
       </c>
@@ -14974,11 +15494,26 @@
         <f t="shared" si="19"/>
         <v>21.157897500000001</v>
       </c>
-      <c r="Y100" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="101" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y100">
+        <v>45.222681713314692</v>
+      </c>
+      <c r="Z100">
+        <v>12.565211489981763</v>
+      </c>
+      <c r="AA100" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB100">
+        <v>3.6091769342682873</v>
+      </c>
+      <c r="AC100">
+        <v>-19.910001101994478</v>
+      </c>
+      <c r="AD100">
+        <v>9.3532259146514782</v>
+      </c>
+    </row>
+    <row r="101" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A101" s="6">
         <v>253</v>
       </c>
@@ -15047,11 +15582,26 @@
         <f t="shared" si="19"/>
         <v>17.923641176470586</v>
       </c>
-      <c r="Y101" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="102" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y101">
+        <v>46.163168599444994</v>
+      </c>
+      <c r="Z101">
+        <v>12.774420096209141</v>
+      </c>
+      <c r="AA101" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB101">
+        <v>3.6137193118569892</v>
+      </c>
+      <c r="AC101">
+        <v>-19.421493201875936</v>
+      </c>
+      <c r="AD101">
+        <v>8.6385141480541829</v>
+      </c>
+    </row>
+    <row r="102" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A102" s="6">
         <v>254</v>
       </c>
@@ -15120,11 +15670,26 @@
         <f t="shared" si="19"/>
         <v>33.232735384615381</v>
       </c>
-      <c r="Y102" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="103" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y102">
+        <v>47.442889543028222</v>
+      </c>
+      <c r="Z102">
+        <v>14.375228920273537</v>
+      </c>
+      <c r="AA102" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB102">
+        <v>3.3003223674663724</v>
+      </c>
+      <c r="AC102">
+        <v>-18.349573003865309</v>
+      </c>
+      <c r="AD102">
+        <v>8.1024803231062119</v>
+      </c>
+    </row>
+    <row r="103" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A103" s="6">
         <v>255</v>
       </c>
@@ -15193,11 +15758,26 @@
         <f t="shared" si="19"/>
         <v>11.14336384615385</v>
       </c>
-      <c r="Y103" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="104" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y103">
+        <v>38.904014858420233</v>
+      </c>
+      <c r="Z103">
+        <v>10.939762881470784</v>
+      </c>
+      <c r="AA103" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB103">
+        <v>3.5562027513698564</v>
+      </c>
+      <c r="AC103">
+        <v>-17.932992647322507</v>
+      </c>
+      <c r="AD103">
+        <v>7.988388719998019</v>
+      </c>
+    </row>
+    <row r="104" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A104" s="6">
         <v>256</v>
       </c>
@@ -15267,11 +15847,26 @@
         <f t="shared" si="19"/>
         <v>31.235702264150948</v>
       </c>
-      <c r="Y104" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="105" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y104">
+        <v>48.495959375707677</v>
+      </c>
+      <c r="Z104">
+        <v>14.251548282428933</v>
+      </c>
+      <c r="AA104" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB104">
+        <v>3.4028554943394802</v>
+      </c>
+      <c r="AC104">
+        <v>-19.588325143225212</v>
+      </c>
+      <c r="AD104">
+        <v>7.9028200176668761</v>
+      </c>
+    </row>
+    <row r="105" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A105" s="6">
         <v>257</v>
       </c>
@@ -15340,11 +15935,26 @@
         <f t="shared" si="19"/>
         <v>28.063069811320762</v>
       </c>
-      <c r="Y105" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="106" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y105">
+        <v>46.412911537766028</v>
+      </c>
+      <c r="Z105">
+        <v>14.110624967783902</v>
+      </c>
+      <c r="AA105" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB105">
+        <v>3.2892172844031906</v>
+      </c>
+      <c r="AC105">
+        <v>-18.718201664690959</v>
+      </c>
+      <c r="AD105">
+        <v>8.7122802707534444</v>
+      </c>
+    </row>
+    <row r="106" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A106" s="6">
         <v>258</v>
       </c>
@@ -15413,11 +16023,26 @@
         <f t="shared" si="19"/>
         <v>44.935706037735855</v>
       </c>
-      <c r="Y106" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="107" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y106">
+        <v>47.291687585801782</v>
+      </c>
+      <c r="Z106">
+        <v>12.328436616349821</v>
+      </c>
+      <c r="AA106" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB106">
+        <v>3.8359841606424068</v>
+      </c>
+      <c r="AC106">
+        <v>-18.828090967376113</v>
+      </c>
+      <c r="AD106">
+        <v>8.1349374170938873</v>
+      </c>
+    </row>
+    <row r="107" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A107" s="6">
         <v>259</v>
       </c>
@@ -15486,11 +16111,11 @@
         <f t="shared" si="19"/>
         <v>12.044753333333333</v>
       </c>
-      <c r="Y107" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="108" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA107" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="108" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A108" s="6">
         <v>260</v>
       </c>
@@ -15559,11 +16184,26 @@
         <f t="shared" si="19"/>
         <v>59.83869927272729</v>
       </c>
-      <c r="Y108" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="109" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y108">
+        <v>48.456742250290766</v>
+      </c>
+      <c r="Z108">
+        <v>14.381520119992919</v>
+      </c>
+      <c r="AA108" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB108">
+        <v>3.3693755490372062</v>
+      </c>
+      <c r="AC108" s="8">
+        <v>-19.185730697933245</v>
+      </c>
+      <c r="AD108">
+        <v>8.1447729001204543</v>
+      </c>
+    </row>
+    <row r="109" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A109" s="6">
         <v>261</v>
       </c>
@@ -15632,11 +16272,26 @@
         <f t="shared" si="19"/>
         <v>25.986443333333334</v>
       </c>
-      <c r="Y109" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="110" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y109">
+        <v>42.527922033242341</v>
+      </c>
+      <c r="Z109">
+        <v>11.075150315543558</v>
+      </c>
+      <c r="AA109" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB109">
+        <v>3.8399408424783181</v>
+      </c>
+      <c r="AC109" s="8">
+        <v>-18.767152354068891</v>
+      </c>
+      <c r="AD109">
+        <v>8.5726164117761758</v>
+      </c>
+    </row>
+    <row r="110" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A110" s="6">
         <v>262</v>
       </c>
@@ -15705,11 +16360,26 @@
         <f t="shared" si="19"/>
         <v>61.071013928571411</v>
       </c>
-      <c r="Y110" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="111" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y110">
+        <v>50.499678753364485</v>
+      </c>
+      <c r="Z110">
+        <v>13.613851459123676</v>
+      </c>
+      <c r="AA110" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB110">
+        <v>3.7094336532899961</v>
+      </c>
+      <c r="AC110" s="8">
+        <v>-17.944980571251797</v>
+      </c>
+      <c r="AD110">
+        <v>9.6348485786455509</v>
+      </c>
+    </row>
+    <row r="111" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A111" s="6">
         <v>263</v>
       </c>
@@ -15778,11 +16448,26 @@
         <f t="shared" si="19"/>
         <v>15.768761052631577</v>
       </c>
-      <c r="Y111" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="112" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y111">
+        <v>48.099677215333443</v>
+      </c>
+      <c r="Z111">
+        <v>14.11218685713753</v>
+      </c>
+      <c r="AA111" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB111">
+        <v>3.4083787085774051</v>
+      </c>
+      <c r="AC111" s="8">
+        <v>-18.197725967427644</v>
+      </c>
+      <c r="AD111">
+        <v>8.1634603178709337</v>
+      </c>
+    </row>
+    <row r="112" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A112" s="6">
         <v>264</v>
       </c>
@@ -15851,11 +16536,26 @@
         <f t="shared" si="19"/>
         <v>11.819311071428572</v>
       </c>
-      <c r="Y112" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="113" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y112">
+        <v>45.716611686129617</v>
+      </c>
+      <c r="Z112">
+        <v>13.751719266610424</v>
+      </c>
+      <c r="AA112" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB112">
+        <v>3.3244288077586694</v>
+      </c>
+      <c r="AC112" s="8">
+        <v>-17.961963463484956</v>
+      </c>
+      <c r="AD112">
+        <v>8.3945941689952903</v>
+      </c>
+    </row>
+    <row r="113" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A113" s="6">
         <v>265</v>
       </c>
@@ -15924,11 +16624,26 @@
         <f t="shared" si="19"/>
         <v>23.467045263157893</v>
       </c>
-      <c r="Y113" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="114" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y113">
+        <v>47.163659826966075</v>
+      </c>
+      <c r="Z113">
+        <v>12.777978046731738</v>
+      </c>
+      <c r="AA113" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB113">
+        <v>3.6910111798970626</v>
+      </c>
+      <c r="AC113" s="8">
+        <v>-19.270645159099047</v>
+      </c>
+      <c r="AD113">
+        <v>9.8177885629397217</v>
+      </c>
+    </row>
+    <row r="114" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A114" s="6">
         <v>266</v>
       </c>
@@ -15993,11 +16708,11 @@
         <f t="shared" si="19"/>
         <v>0.57416400000000023</v>
       </c>
-      <c r="Y114" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="115" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA114" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="115" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A115" s="6">
         <v>267</v>
       </c>
@@ -16062,11 +16777,11 @@
         <f t="shared" si="19"/>
         <v>-11.198234042553196</v>
       </c>
-      <c r="Y115" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="116" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA115" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="116" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A116" s="6">
         <v>268</v>
       </c>
@@ -16133,11 +16848,11 @@
         <f t="shared" si="19"/>
         <v>1713.7757727272731</v>
       </c>
-      <c r="Y116" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="117" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA116" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="117" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A117" s="6">
         <v>269</v>
       </c>
@@ -16203,11 +16918,11 @@
         <f t="shared" si="19"/>
         <v>3834.9456818181829</v>
       </c>
-      <c r="Y117" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="118" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA117" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="118" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A118" s="6">
         <v>270</v>
       </c>
@@ -16273,11 +16988,26 @@
         <f t="shared" si="19"/>
         <v>49.092815454545445</v>
       </c>
-      <c r="Y118" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="119" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y118">
+        <v>38.528017779695212</v>
+      </c>
+      <c r="Z118">
+        <v>11.684147103135688</v>
+      </c>
+      <c r="AA118" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB118">
+        <v>3.2974608621073767</v>
+      </c>
+      <c r="AC118">
+        <v>-19.374540499819553</v>
+      </c>
+      <c r="AD118">
+        <v>9.4627276256806052</v>
+      </c>
+    </row>
+    <row r="119" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A119" s="6">
         <v>271</v>
       </c>
@@ -16343,11 +17073,26 @@
         <f t="shared" si="19"/>
         <v>144.46508294117649</v>
       </c>
-      <c r="Y119" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="120" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y119">
+        <v>44.830058985901388</v>
+      </c>
+      <c r="Z119">
+        <v>11.901785151830669</v>
+      </c>
+      <c r="AA119" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB119">
+        <v>3.7666667994763681</v>
+      </c>
+      <c r="AC119">
+        <v>-22.103791181054437</v>
+      </c>
+      <c r="AD119">
+        <v>11.333436497333894</v>
+      </c>
+    </row>
+    <row r="120" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A120" s="6">
         <v>272</v>
       </c>
@@ -16414,11 +17159,26 @@
         <f t="shared" si="19"/>
         <v>106.24928294117646</v>
       </c>
-      <c r="Y120" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="121" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y120">
+        <v>48.226425748934403</v>
+      </c>
+      <c r="Z120">
+        <v>10.664345066825575</v>
+      </c>
+      <c r="AA120" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB120">
+        <v>4.5222116732659163</v>
+      </c>
+      <c r="AC120">
+        <v>-18.245677663144804</v>
+      </c>
+      <c r="AD120">
+        <v>10.690195907396328</v>
+      </c>
+    </row>
+    <row r="121" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A121" s="6">
         <v>273</v>
       </c>
@@ -16486,11 +17246,26 @@
         <f t="shared" si="19"/>
         <v>184.32226058823528</v>
       </c>
-      <c r="Y121" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="122" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y121">
+        <v>46.80955726952849</v>
+      </c>
+      <c r="Z121">
+        <v>12.787587579788466</v>
+      </c>
+      <c r="AA121" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB121">
+        <v>3.6606505735550718</v>
+      </c>
+      <c r="AC121">
+        <v>-22.266627147760616</v>
+      </c>
+      <c r="AD121">
+        <v>11.608830022077806</v>
+      </c>
+    </row>
+    <row r="122" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A122" s="6">
         <v>274</v>
       </c>
@@ -16558,11 +17333,26 @@
         <f t="shared" si="19"/>
         <v>84.593662941176461</v>
       </c>
-      <c r="Y122" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="123" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y122">
+        <v>44.139915199511876</v>
+      </c>
+      <c r="Z122">
+        <v>12.617039210032626</v>
+      </c>
+      <c r="AA122" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB122">
+        <v>3.4984368729244628</v>
+      </c>
+      <c r="AC122">
+        <v>-19.478435840540062</v>
+      </c>
+      <c r="AD122">
+        <v>11.457363583468654</v>
+      </c>
+    </row>
+    <row r="123" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A123" s="6">
         <v>275</v>
       </c>
@@ -16629,11 +17419,26 @@
         <f t="shared" si="19"/>
         <v>145.15050529411764</v>
       </c>
-      <c r="Y123" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="124" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y123">
+        <v>44.04375030725928</v>
+      </c>
+      <c r="Z123">
+        <v>12.262638450025605</v>
+      </c>
+      <c r="AA123" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB123">
+        <v>3.5917025921258663</v>
+      </c>
+      <c r="AC123">
+        <v>-15.226718820285427</v>
+      </c>
+      <c r="AD123">
+        <v>9.2148734534110854</v>
+      </c>
+    </row>
+    <row r="124" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A124" s="6">
         <v>276</v>
       </c>
@@ -16701,11 +17506,26 @@
         <f t="shared" si="19"/>
         <v>191.07337235294119</v>
       </c>
-      <c r="Y124" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="125" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y124">
+        <v>49.669454425579339</v>
+      </c>
+      <c r="Z124">
+        <v>12.958574296825196</v>
+      </c>
+      <c r="AA124" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB124">
+        <v>3.8329412856588845</v>
+      </c>
+      <c r="AC124">
+        <v>-26.521341148997575</v>
+      </c>
+      <c r="AD124">
+        <v>13.488390828455005</v>
+      </c>
+    </row>
+    <row r="125" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A125" s="6">
         <v>277</v>
       </c>
@@ -16773,11 +17593,26 @@
         <f t="shared" si="19"/>
         <v>113.29297941176468</v>
       </c>
-      <c r="Y125" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="126" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y125">
+        <v>47.739124117278834</v>
+      </c>
+      <c r="Z125">
+        <v>13.00332994533488</v>
+      </c>
+      <c r="AA125" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB125">
+        <v>3.6712999145581082</v>
+      </c>
+      <c r="AC125">
+        <v>-20.866038035355309</v>
+      </c>
+      <c r="AD125">
+        <v>11.191805541751311</v>
+      </c>
+    </row>
+    <row r="126" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A126" s="6">
         <v>278</v>
       </c>
@@ -16844,11 +17679,26 @@
         <f t="shared" si="19"/>
         <v>193.30209352941179</v>
       </c>
-      <c r="Y126" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="127" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y126">
+        <v>44.20551965286932</v>
+      </c>
+      <c r="Z126">
+        <v>11.695709023089174</v>
+      </c>
+      <c r="AA126" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB126">
+        <v>3.7796357249997117</v>
+      </c>
+      <c r="AC126">
+        <v>-21.956939112920644</v>
+      </c>
+      <c r="AD126">
+        <v>7.493663923761634</v>
+      </c>
+    </row>
+    <row r="127" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A127" s="6">
         <v>279</v>
       </c>
@@ -16915,11 +17765,26 @@
         <f t="shared" si="19"/>
         <v>142.91254557692309</v>
       </c>
-      <c r="Y127" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="128" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y127">
+        <v>52.170134348509578</v>
+      </c>
+      <c r="Z127">
+        <v>11.135309357323026</v>
+      </c>
+      <c r="AA127" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB127">
+        <v>4.6851086641971387</v>
+      </c>
+      <c r="AC127">
+        <v>-26.197667202906761</v>
+      </c>
+      <c r="AD127">
+        <v>5.0072538146451713</v>
+      </c>
+    </row>
+    <row r="128" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A128" s="6">
         <v>280</v>
       </c>
@@ -16986,11 +17851,26 @@
         <f t="shared" si="19"/>
         <v>103.55464557692309</v>
       </c>
-      <c r="Y128" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="129" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y128">
+        <v>43.893163876723555</v>
+      </c>
+      <c r="Z128">
+        <v>12.245561308853221</v>
+      </c>
+      <c r="AA128" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB128">
+        <v>3.5844142028009731</v>
+      </c>
+      <c r="AC128">
+        <v>-23.498386331495098</v>
+      </c>
+      <c r="AD128">
+        <v>12.001265794837881</v>
+      </c>
+    </row>
+    <row r="129" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A129" s="6">
         <v>281</v>
       </c>
@@ -17057,11 +17937,26 @@
         <f t="shared" si="19"/>
         <v>83.478322941176486</v>
       </c>
-      <c r="Y129" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="130" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y129">
+        <v>43.387639561216638</v>
+      </c>
+      <c r="Z129">
+        <v>13.056967864961122</v>
+      </c>
+      <c r="AA129" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB129">
+        <v>3.3229490958348031</v>
+      </c>
+      <c r="AC129">
+        <v>-21.178723051177606</v>
+      </c>
+      <c r="AD129">
+        <v>12.223547711238323</v>
+      </c>
+    </row>
+    <row r="130" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A130" s="6">
         <v>282</v>
       </c>
@@ -17129,11 +18024,11 @@
         <f t="shared" si="19"/>
         <v>119.52395823529412</v>
       </c>
-      <c r="Y130" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="131" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA130" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="131" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A131" s="6">
         <v>283</v>
       </c>
@@ -17201,11 +18096,26 @@
         <f t="shared" ref="U131:U160" si="30">(T131/J131*60)/G131</f>
         <v>124.26894540000001</v>
       </c>
-      <c r="Y131" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="132" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y131">
+        <v>44.00341777957469</v>
+      </c>
+      <c r="Z131" s="8">
+        <v>12.317630810143008</v>
+      </c>
+      <c r="AA131" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB131">
+        <v>3.572392975387757</v>
+      </c>
+      <c r="AC131" s="8">
+        <v>-24.232646672164076</v>
+      </c>
+      <c r="AD131" s="8">
+        <v>9.7312363123059207</v>
+      </c>
+    </row>
+    <row r="132" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A132" s="6">
         <v>284</v>
       </c>
@@ -17273,11 +18183,11 @@
         <f t="shared" si="30"/>
         <v>119.16882882352942</v>
       </c>
-      <c r="Y132" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="133" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA132" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="133" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A133" s="6">
         <v>285</v>
       </c>
@@ -17345,11 +18255,11 @@
         <f t="shared" si="30"/>
         <v>203.42328176470591</v>
       </c>
-      <c r="Y133" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="134" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA133" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="134" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A134" s="6">
         <v>286</v>
       </c>
@@ -17417,11 +18327,26 @@
         <f t="shared" si="30"/>
         <v>104.34217588235296</v>
       </c>
-      <c r="Y134" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="135" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y134">
+        <v>48.054086114886189</v>
+      </c>
+      <c r="Z134">
+        <v>12.834374607920509</v>
+      </c>
+      <c r="AA134" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB134">
+        <v>3.7441704471700907</v>
+      </c>
+      <c r="AC134" s="8">
+        <v>-22.144749921146175</v>
+      </c>
+      <c r="AD134" s="8">
+        <v>11.57047163827419</v>
+      </c>
+    </row>
+    <row r="135" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A135" s="6">
         <v>287</v>
       </c>
@@ -17489,11 +18414,26 @@
         <f t="shared" si="30"/>
         <v>134.353666</v>
       </c>
-      <c r="Y135" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="136" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y135">
+        <v>50.114169135822124</v>
+      </c>
+      <c r="Z135">
+        <v>14.070076092226097</v>
+      </c>
+      <c r="AA135" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB135">
+        <v>3.5617553741241572</v>
+      </c>
+      <c r="AC135" s="8">
+        <v>-19.296618994279171</v>
+      </c>
+      <c r="AD135" s="8">
+        <v>10.257434654227325</v>
+      </c>
+    </row>
+    <row r="136" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A136" s="6">
         <v>288</v>
       </c>
@@ -17561,11 +18501,26 @@
         <f t="shared" si="30"/>
         <v>80.051112391304358</v>
       </c>
-      <c r="Y136" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="137" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y136">
+        <v>43.119970224196379</v>
+      </c>
+      <c r="Z136">
+        <v>12.904828212048425</v>
+      </c>
+      <c r="AA136" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB136">
+        <v>3.3413827379691874</v>
+      </c>
+      <c r="AC136" s="8">
+        <v>-24.18469497644692</v>
+      </c>
+      <c r="AD136" s="8">
+        <v>13.585762110418031</v>
+      </c>
+    </row>
+    <row r="137" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A137" s="6">
         <v>289</v>
       </c>
@@ -17633,11 +18588,11 @@
         <f t="shared" si="30"/>
         <v>5682.3601499999986</v>
       </c>
-      <c r="Y137" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="138" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA137" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="138" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A138" s="6">
         <v>290</v>
       </c>
@@ -17704,11 +18659,11 @@
         <f t="shared" si="30"/>
         <v>553.217895</v>
       </c>
-      <c r="Y138" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="139" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA138" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="139" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A139" s="6">
         <v>291</v>
       </c>
@@ -17775,11 +18730,26 @@
         <f t="shared" si="30"/>
         <v>1083.0215600000001</v>
       </c>
-      <c r="Y139" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="140" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y139" s="8">
+        <v>42.591594406979894</v>
+      </c>
+      <c r="Z139">
+        <v>12.418261403679463</v>
+      </c>
+      <c r="AA139" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB139" s="8">
+        <v>3.429755021452539</v>
+      </c>
+      <c r="AC139" s="8">
+        <v>-14.280671823532341</v>
+      </c>
+      <c r="AD139" s="8">
+        <v>8.7663754273995718</v>
+      </c>
+    </row>
+    <row r="140" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A140" s="6">
         <v>292</v>
       </c>
@@ -17847,11 +18817,26 @@
         <f t="shared" si="30"/>
         <v>244.42652785714284</v>
       </c>
-      <c r="Y140" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="141" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y140" s="8">
+        <v>46.888005736622112</v>
+      </c>
+      <c r="Z140">
+        <v>11.795986793222362</v>
+      </c>
+      <c r="AA140" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB140" s="8">
+        <v>3.9749116846725046</v>
+      </c>
+      <c r="AC140" s="8">
+        <v>-13.498459787146206</v>
+      </c>
+      <c r="AD140" s="8">
+        <v>9.0545550800780212</v>
+      </c>
+    </row>
+    <row r="141" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A141" s="6">
         <v>293</v>
       </c>
@@ -17919,11 +18904,26 @@
         <f t="shared" si="30"/>
         <v>198.44886348837204</v>
       </c>
-      <c r="Y141" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="142" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y141" s="8">
+        <v>42.382009347829879</v>
+      </c>
+      <c r="Z141">
+        <v>13.028234894321105</v>
+      </c>
+      <c r="AA141" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB141" s="8">
+        <v>3.2530891323047784</v>
+      </c>
+      <c r="AC141" s="8">
+        <v>-16.520415610987907</v>
+      </c>
+      <c r="AD141" s="8">
+        <v>9.5384608449851811</v>
+      </c>
+    </row>
+    <row r="142" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A142" s="6">
         <v>294</v>
       </c>
@@ -17990,11 +18990,11 @@
         <f t="shared" si="30"/>
         <v>3599.6960297872351</v>
       </c>
-      <c r="Y142" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="143" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA142" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="143" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A143" s="6">
         <v>295</v>
       </c>
@@ -18061,11 +19061,11 @@
         <f t="shared" si="30"/>
         <v>2903.4083936170214</v>
       </c>
-      <c r="Y143" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="144" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA143" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="144" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A144" s="6">
         <v>296</v>
       </c>
@@ -18131,11 +19131,11 @@
         <f t="shared" si="30"/>
         <v>4193.8370999999997</v>
       </c>
-      <c r="Y144" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="145" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA144" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="145" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A145" s="6">
         <v>297</v>
       </c>
@@ -18201,11 +19201,11 @@
         <f t="shared" si="30"/>
         <v>2164.3325162790698</v>
       </c>
-      <c r="Y145" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="146" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA145" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="146" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A146" s="6">
         <v>298</v>
       </c>
@@ -18272,11 +19272,11 @@
         <f t="shared" si="30"/>
         <v>3951.5653378378379</v>
       </c>
-      <c r="Y146" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="147" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA146" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="147" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A147" s="6">
         <v>299</v>
       </c>
@@ -18343,11 +19343,11 @@
         <f t="shared" si="30"/>
         <v>3586.4261447368422</v>
       </c>
-      <c r="Y147" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="148" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA147" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="148" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A148" s="6">
         <v>300</v>
       </c>
@@ -18414,11 +19414,11 @@
         <f t="shared" si="30"/>
         <v>2159.0275657894731</v>
       </c>
-      <c r="Y148" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="149" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA148" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="149" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A149" s="6">
         <v>301</v>
       </c>
@@ -18485,11 +19485,11 @@
         <f t="shared" si="30"/>
         <v>3831.5313088235289</v>
       </c>
-      <c r="Y149" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="150" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA149" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="150" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A150" s="6">
         <v>302</v>
       </c>
@@ -18556,11 +19556,11 @@
         <f t="shared" si="30"/>
         <v>2259.0204187499994</v>
       </c>
-      <c r="Y150" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="151" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA150" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="151" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A151" s="6">
         <v>303</v>
       </c>
@@ -18627,11 +19627,11 @@
         <f t="shared" si="30"/>
         <v>2818.8989482758634</v>
       </c>
-      <c r="Y151" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="152" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA151" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="152" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A152" s="6">
         <v>304</v>
       </c>
@@ -18697,11 +19697,11 @@
         <f t="shared" si="30"/>
         <v>3685.5421500000002</v>
       </c>
-      <c r="Y152" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="153" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA152" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="153" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A153" s="6">
         <v>305</v>
       </c>
@@ -18767,11 +19767,11 @@
         <f t="shared" si="30"/>
         <v>4259.01325</v>
       </c>
-      <c r="Y153" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="154" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA153" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="154" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A154" s="6">
         <v>306</v>
       </c>
@@ -18837,11 +19837,11 @@
         <f t="shared" si="30"/>
         <v>2362.2854275862073</v>
       </c>
-      <c r="Y154" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="155" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA154" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="155" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A155" s="6">
         <v>307</v>
       </c>
@@ -18907,11 +19907,11 @@
         <f t="shared" si="30"/>
         <v>3454.7240192307695</v>
       </c>
-      <c r="Y155" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="156" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA155" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="156" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A156" s="6">
         <v>308</v>
       </c>
@@ -18977,11 +19977,11 @@
         <f t="shared" si="30"/>
         <v>4748.5728600000011</v>
       </c>
-      <c r="Y156" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="157" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA156" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="157" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A157" s="6">
         <v>309</v>
       </c>
@@ -19047,11 +20047,11 @@
         <f t="shared" si="30"/>
         <v>5132.5070999999989</v>
       </c>
-      <c r="Y157" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="158" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA157" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="158" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A158" s="6">
         <v>310</v>
       </c>
@@ -19118,11 +20118,11 @@
         <f t="shared" si="30"/>
         <v>2839.0260960000005</v>
       </c>
-      <c r="Y158" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="159" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA158" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="159" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A159" s="6">
         <v>311</v>
       </c>
@@ -19187,11 +20187,11 @@
         <f t="shared" si="30"/>
         <v>13.800575000000004</v>
       </c>
-      <c r="Y159" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="160" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA159" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="160" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A160" s="6">
         <v>312</v>
       </c>
@@ -19256,7 +20256,7 @@
         <f t="shared" si="30"/>
         <v>-1.0139197959183675</v>
       </c>
-      <c r="Y160" s="6" t="s">
+      <c r="AA160" s="6" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
made new tables and modified some figures
</commit_message>
<xml_diff>
--- a/data/2022-03-03_LakeErie_Mastersheet.xlsx
+++ b/data/2022-03-03_LakeErie_Mastersheet.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://trentu-my.sharepoint.com/personal/sandraklemet_trentu_ca/Documents/Documents/Etudes/Trent/Xenopoulos lab/Projects/LakeErie_animal-excretion/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="350" documentId="13_ncr:1_{EA2E9A16-F367-47E5-9F32-F761EF32E94C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD75D51B-6930-496E-94B3-ADA71AE56E1A}"/>
+  <xr:revisionPtr revIDLastSave="460" documentId="13_ncr:1_{EA2E9A16-F367-47E5-9F32-F761EF32E94C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{628324BC-6800-441E-BA77-8A9F29459029}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FCD5901F-55C5-46A6-83E9-A175C073FB2F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="6" xr2:uid="{FCD5901F-55C5-46A6-83E9-A175C073FB2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Fishing and Environmental data" sheetId="3" r:id="rId1"/>
     <sheet name="Fish and mussel sampling" sheetId="1" r:id="rId2"/>
-    <sheet name="Biomass estimates" sheetId="5" r:id="rId3"/>
-    <sheet name="Column headings" sheetId="4" r:id="rId4"/>
-    <sheet name="21 08 26 Lake Erie Mastersheet" sheetId="2" r:id="rId5"/>
+    <sheet name="Fish_biomass_estimates" sheetId="5" r:id="rId3"/>
+    <sheet name="Dreissenid_biomass_estimates" sheetId="6" r:id="rId4"/>
+    <sheet name="WesternBasin_biomass" sheetId="7" r:id="rId5"/>
+    <sheet name="Column headings" sheetId="4" r:id="rId6"/>
+    <sheet name="21 08 26 Lake Erie Mastersheet" sheetId="2" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'21 08 26 Lake Erie Mastersheet'!$A$1:$CJ$160</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'21 08 26 Lake Erie Mastersheet'!$A$1:$CJ$160</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Fish and mussel sampling'!$A$1:$L$160</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2322" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2351" uniqueCount="223">
   <si>
     <t>Sampling run</t>
   </si>
@@ -685,12 +687,39 @@
   <si>
     <t>for fish, from stable isotopes analyses in Fisk lab - used data based on whole body or muscle analyses. Summer data = collected in Aug. 2019, with YP average of all YP values since only have one individual tested for excretion. Fall data = collected in Oct. 2021. For mussels, used mussel tissue collected from individuals tested in the summer 2021 and analyzed at Trent Water Quality Centre in Feb 2023</t>
   </si>
+  <si>
+    <t>Ref: 500 g/m2 = 3.6cm</t>
+  </si>
+  <si>
+    <t>Biomass (g/m2)</t>
+  </si>
+  <si>
+    <t>Species.code</t>
+  </si>
+  <si>
+    <t>DM</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Fish</t>
+  </si>
+  <si>
+    <t>Dreissenid</t>
+  </si>
+  <si>
+    <t>Biomass (kg/ha) SD</t>
+  </si>
+  <si>
+    <t>Biomass (g/m2) SD</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -720,6 +749,19 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -742,7 +784,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -757,6 +799,8 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -775,10 +819,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -816,7 +864,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -922,7 +970,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1064,7 +1112,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1074,7 +1122,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BEA8862-2595-4F8C-BCE3-C83A0E339B61}">
   <dimension ref="A1:BO8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
@@ -8123,7 +8171,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8475,6 +8523,328 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1DD69A6-9758-46F5-A03C-8A6B27428E10}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="8">
+        <v>2019</v>
+      </c>
+      <c r="B2">
+        <f>2.25/3.6*500</f>
+        <v>312.5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="9">
+        <v>2014</v>
+      </c>
+      <c r="B3">
+        <f>3.1/3.6*500</f>
+        <v>430.5555555555556</v>
+      </c>
+      <c r="C3" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="9">
+        <v>2011</v>
+      </c>
+      <c r="B4">
+        <f>1.4/3.6*500</f>
+        <v>194.44444444444443</v>
+      </c>
+      <c r="C4" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="9">
+        <v>2004</v>
+      </c>
+      <c r="B5">
+        <f>2.6/3.6*500</f>
+        <v>361.11111111111109</v>
+      </c>
+      <c r="C5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="9">
+        <v>2002</v>
+      </c>
+      <c r="B6">
+        <f>4.7/3.6*500</f>
+        <v>652.77777777777783</v>
+      </c>
+      <c r="C6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="9">
+        <v>1998</v>
+      </c>
+      <c r="B7">
+        <f>2.75/3.6*500</f>
+        <v>381.9444444444444</v>
+      </c>
+      <c r="C7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="9">
+        <v>1993</v>
+      </c>
+      <c r="B8">
+        <f>2/3.6*500</f>
+        <v>277.77777777777777</v>
+      </c>
+      <c r="C8" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="9">
+        <v>1992</v>
+      </c>
+      <c r="B9">
+        <f>1.3/3.6*500</f>
+        <v>180.55555555555554</v>
+      </c>
+      <c r="C9" t="s">
+        <v>217</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C1934CC-AF7C-4B16-A1BA-6A4CD2D5F7CF}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>2020</v>
+      </c>
+      <c r="B2">
+        <v>99</v>
+      </c>
+      <c r="D2">
+        <v>117</v>
+      </c>
+      <c r="F2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2019</v>
+      </c>
+      <c r="B3">
+        <f>AVERAGE(136,96)</f>
+        <v>116</v>
+      </c>
+      <c r="D3">
+        <f>AVERAGE(108,102)</f>
+        <v>105</v>
+      </c>
+      <c r="F3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>2018</v>
+      </c>
+      <c r="B4">
+        <v>88</v>
+      </c>
+      <c r="D4">
+        <v>52</v>
+      </c>
+      <c r="F4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>2017</v>
+      </c>
+      <c r="B5">
+        <f>AVERAGE(96,46)</f>
+        <v>71</v>
+      </c>
+      <c r="D5">
+        <f>AVERAGE(69,43)</f>
+        <v>56</v>
+      </c>
+      <c r="F5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>2016</v>
+      </c>
+      <c r="B6">
+        <f>AVERAGE(101, 74)</f>
+        <v>87.5</v>
+      </c>
+      <c r="D6">
+        <f>AVERAGE(75, 57)</f>
+        <v>66</v>
+      </c>
+      <c r="F6" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>2015</v>
+      </c>
+      <c r="B7">
+        <f>AVERAGE(122, 86)</f>
+        <v>104</v>
+      </c>
+      <c r="D7">
+        <f>AVERAGE(100, 66)</f>
+        <v>83</v>
+      </c>
+      <c r="F7" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>2014</v>
+      </c>
+      <c r="B8">
+        <f>AVERAGE(194, 178)</f>
+        <v>186</v>
+      </c>
+      <c r="D8">
+        <f>AVERAGE(173, 113)</f>
+        <v>143</v>
+      </c>
+      <c r="F8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>2013</v>
+      </c>
+      <c r="B9">
+        <f>AVERAGE(310, 235)</f>
+        <v>272.5</v>
+      </c>
+      <c r="D9">
+        <f>AVERAGE(249, 154)</f>
+        <v>201.5</v>
+      </c>
+      <c r="F9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>2019</v>
+      </c>
+      <c r="C10">
+        <v>48</v>
+      </c>
+      <c r="E10">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="F10" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>2014</v>
+      </c>
+      <c r="C11">
+        <f>1.6/3.2*500</f>
+        <v>250</v>
+      </c>
+      <c r="F11" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>2011</v>
+      </c>
+      <c r="C12">
+        <f>2.7/3.2*500</f>
+        <v>421.875</v>
+      </c>
+      <c r="F12" t="s">
+        <v>220</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCB797C5-CB47-4805-AD51-BAF5F7220E5D}">
   <dimension ref="A1:AF17"/>
   <sheetViews>
@@ -8736,15 +9106,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4782880F-19F5-4C97-B687-8149361B0730}">
   <dimension ref="A1:CJ160"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="R21" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AN44" sqref="AN44"/>
+      <selection pane="bottomRight" activeCell="AE31" sqref="AE31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9106,8 +9476,17 @@
         <f>(Z2/J2*60)/G2</f>
         <v>6537.8599495402977</v>
       </c>
+      <c r="AB2">
+        <v>48.387730230000003</v>
+      </c>
+      <c r="AC2">
+        <v>14.85303817</v>
+      </c>
       <c r="AD2" t="s">
         <v>31</v>
+      </c>
+      <c r="AE2">
+        <v>3.2577665040000001</v>
       </c>
       <c r="AF2" t="s">
         <v>31</v>
@@ -9372,11 +9751,17 @@
         <f t="shared" ref="AA3:AA66" si="8">(Z3/J3*60)/G3</f>
         <v>4989.2799861942904</v>
       </c>
+      <c r="AB3">
+        <v>48.145931959999999</v>
+      </c>
+      <c r="AC3">
+        <v>14.62314237</v>
+      </c>
       <c r="AD3" t="s">
         <v>31</v>
       </c>
       <c r="AE3">
-        <v>4.9547660021985802</v>
+        <v>3.2924477350000001</v>
       </c>
       <c r="AF3" t="s">
         <v>31</v>
@@ -9641,8 +10026,17 @@
         <f t="shared" si="8"/>
         <v>3670.9015726696243</v>
       </c>
+      <c r="AB4">
+        <v>50.442654920000003</v>
+      </c>
+      <c r="AC4">
+        <v>13.864247049999999</v>
+      </c>
       <c r="AD4" t="s">
         <v>31</v>
+      </c>
+      <c r="AE4">
+        <v>3.6383263170000002</v>
       </c>
       <c r="AF4" t="s">
         <v>31</v>
@@ -9907,11 +10301,17 @@
         <f t="shared" si="8"/>
         <v>2432.2891785802917</v>
       </c>
+      <c r="AB5">
+        <v>49.353448210000003</v>
+      </c>
+      <c r="AC5">
+        <v>14.41409494</v>
+      </c>
       <c r="AD5" t="s">
         <v>31</v>
       </c>
       <c r="AE5">
-        <v>4.7499695394714312</v>
+        <v>3.4239713570000001</v>
       </c>
       <c r="AF5" t="s">
         <v>31</v>
@@ -10176,11 +10576,17 @@
         <f t="shared" si="8"/>
         <v>2235.0599670628344</v>
       </c>
+      <c r="AB6">
+        <v>45.834344119999997</v>
+      </c>
+      <c r="AC6">
+        <v>13.68383482</v>
+      </c>
       <c r="AD6" t="s">
         <v>31</v>
       </c>
       <c r="AE6">
-        <v>3.2918023079999998</v>
+        <v>3.3495248009999998</v>
       </c>
       <c r="AF6" t="s">
         <v>31</v>
@@ -10189,10 +10595,10 @@
         <v>31</v>
       </c>
       <c r="AH6">
-        <v>-23.199938060000001</v>
+        <v>-23.99557239</v>
       </c>
       <c r="AI6">
-        <v>13.32790164</v>
+        <v>12.90011838</v>
       </c>
       <c r="AJ6" s="7">
         <v>8.51</v>
@@ -10445,11 +10851,17 @@
         <f t="shared" si="8"/>
         <v>1656.2443511485969</v>
       </c>
+      <c r="AB7">
+        <v>45.891883290000003</v>
+      </c>
+      <c r="AC7">
+        <v>14.02760546</v>
+      </c>
       <c r="AD7" t="s">
         <v>31</v>
       </c>
       <c r="AE7">
-        <v>3.4736409730000002</v>
+        <v>3.2715407779999999</v>
       </c>
       <c r="AF7" t="s">
         <v>31</v>
@@ -10458,10 +10870,10 @@
         <v>31</v>
       </c>
       <c r="AH7">
-        <v>-23.750301650000001</v>
+        <v>-23.983607960000001</v>
       </c>
       <c r="AI7">
-        <v>12.46836497</v>
+        <v>12.33139493</v>
       </c>
       <c r="AJ7" s="7">
         <v>8.51</v>
@@ -15387,20 +15799,11 @@
       <c r="AD26" t="s">
         <v>31</v>
       </c>
-      <c r="AE26">
-        <v>3.3495248009999998</v>
-      </c>
       <c r="AF26" t="s">
         <v>31</v>
       </c>
       <c r="AG26" t="s">
         <v>31</v>
-      </c>
-      <c r="AH26">
-        <v>-23.99557239</v>
-      </c>
-      <c r="AI26">
-        <v>12.90011838</v>
       </c>
       <c r="AJ26" s="7">
         <v>8.49</v>
@@ -16734,11 +17137,17 @@
         <f t="shared" si="8"/>
         <v>2842.1206317251458</v>
       </c>
+      <c r="AB31">
+        <v>46.820824039999998</v>
+      </c>
+      <c r="AC31">
+        <v>14.28768788</v>
+      </c>
       <c r="AD31" t="s">
         <v>31</v>
       </c>
       <c r="AE31">
-        <v>3.3357466021111106</v>
+        <v>3.2770049609999998</v>
       </c>
       <c r="AF31" t="s">
         <v>31</v>
@@ -16747,10 +17156,10 @@
         <v>31</v>
       </c>
       <c r="AH31">
-        <v>-23.614508616666669</v>
+        <v>-23.886097759999998</v>
       </c>
       <c r="AI31">
-        <v>13.141214462222223</v>
+        <v>12.58401098</v>
       </c>
       <c r="AJ31" s="7">
         <v>8.49</v>
@@ -17261,20 +17670,11 @@
       <c r="AD33" t="s">
         <v>31</v>
       </c>
-      <c r="AE33">
-        <v>3.2715407779999999</v>
-      </c>
       <c r="AF33" t="s">
         <v>31</v>
       </c>
       <c r="AG33" t="s">
         <v>31</v>
-      </c>
-      <c r="AH33">
-        <v>-23.983607960000001</v>
-      </c>
-      <c r="AI33">
-        <v>12.33139493</v>
       </c>
       <c r="AJ33">
         <v>8.4700000000000006</v>
@@ -17787,6 +18187,12 @@
         <f t="shared" si="8"/>
         <v>15275.106764049448</v>
       </c>
+      <c r="AB35">
+        <v>44.942498649999997</v>
+      </c>
+      <c r="AC35">
+        <v>14.150903189999999</v>
+      </c>
       <c r="AD35" t="s">
         <v>31</v>
       </c>
@@ -18056,6 +18462,12 @@
         <f t="shared" si="8"/>
         <v>19399.629493172204</v>
       </c>
+      <c r="AB36">
+        <v>43.323799899999997</v>
+      </c>
+      <c r="AC36">
+        <v>12.7768157</v>
+      </c>
       <c r="AD36" t="s">
         <v>31</v>
       </c>
@@ -18325,6 +18737,12 @@
         <f t="shared" si="8"/>
         <v>9190.1849384170073</v>
       </c>
+      <c r="AB37">
+        <v>44.376729159999996</v>
+      </c>
+      <c r="AC37">
+        <v>14.06385596</v>
+      </c>
       <c r="AD37" t="s">
         <v>31</v>
       </c>
@@ -18854,14 +19272,29 @@
         <f t="shared" si="8"/>
         <v>2698.909275762624</v>
       </c>
+      <c r="AB39">
+        <v>46.958182299999997</v>
+      </c>
+      <c r="AC39">
+        <v>14.26518907</v>
+      </c>
       <c r="AD39" t="s">
         <v>31</v>
       </c>
+      <c r="AE39">
+        <v>3.2918023079999998</v>
+      </c>
       <c r="AF39" t="s">
         <v>31</v>
       </c>
       <c r="AG39" t="s">
         <v>31</v>
+      </c>
+      <c r="AH39">
+        <v>-23.199938060000001</v>
+      </c>
+      <c r="AI39">
+        <v>13.32790164</v>
       </c>
       <c r="AJ39">
         <v>8.4700000000000006</v>
@@ -19114,14 +19547,29 @@
         <f t="shared" si="8"/>
         <v>3119.5225225396653</v>
       </c>
+      <c r="AB40">
+        <v>47.341653639999997</v>
+      </c>
+      <c r="AC40">
+        <v>13.628827510000001</v>
+      </c>
       <c r="AD40" t="s">
         <v>31</v>
       </c>
+      <c r="AE40">
+        <v>3.4736409730000002</v>
+      </c>
       <c r="AF40" t="s">
         <v>31</v>
       </c>
       <c r="AG40" t="s">
         <v>31</v>
+      </c>
+      <c r="AH40">
+        <v>-23.750301650000001</v>
+      </c>
+      <c r="AI40">
+        <v>12.46836497</v>
       </c>
       <c r="AJ40">
         <v>8.4700000000000006</v>

</xml_diff>

<commit_message>
updated most figures and added new tables
</commit_message>
<xml_diff>
--- a/data/2022-03-03_LakeErie_Mastersheet.xlsx
+++ b/data/2022-03-03_LakeErie_Mastersheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://trentu-my.sharepoint.com/personal/sandraklemet_trentu_ca/Documents/Documents/Etudes/Trent/Xenopoulos lab/Projects/LakeErie_animal-excretion/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="460" documentId="13_ncr:1_{EA2E9A16-F367-47E5-9F32-F761EF32E94C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{628324BC-6800-441E-BA77-8A9F29459029}"/>
+  <xr:revisionPtr revIDLastSave="488" documentId="13_ncr:1_{EA2E9A16-F367-47E5-9F32-F761EF32E94C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{552A0181-A305-432F-B9D4-93FBCBBED485}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="6" xr2:uid="{FCD5901F-55C5-46A6-83E9-A175C073FB2F}"/>
   </bookViews>
@@ -819,10 +819,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
@@ -9114,7 +9110,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AE31" sqref="AE31"/>
+      <selection pane="bottomRight" activeCell="Y35" sqref="Y35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9477,16 +9473,16 @@
         <v>6537.8599495402977</v>
       </c>
       <c r="AB2">
-        <v>48.387730230000003</v>
+        <v>48.130241346153859</v>
       </c>
       <c r="AC2">
-        <v>14.85303817</v>
+        <v>13.736281153307694</v>
       </c>
       <c r="AD2" t="s">
         <v>31</v>
       </c>
       <c r="AE2">
-        <v>3.2577665040000001</v>
+        <v>3.5897974680769233</v>
       </c>
       <c r="AF2" t="s">
         <v>31</v>
@@ -9495,10 +9491,10 @@
         <v>31</v>
       </c>
       <c r="AH2">
-        <v>-23.46392457</v>
+        <v>-23.615299784615388</v>
       </c>
       <c r="AI2">
-        <v>13.6533783</v>
+        <v>12.931454542307693</v>
       </c>
       <c r="AJ2" s="7">
         <v>8.51</v>
@@ -9752,16 +9748,16 @@
         <v>4989.2799861942904</v>
       </c>
       <c r="AB3">
-        <v>48.145931959999999</v>
+        <v>48.130241346153859</v>
       </c>
       <c r="AC3">
-        <v>14.62314237</v>
+        <v>13.736281153307694</v>
       </c>
       <c r="AD3" t="s">
         <v>31</v>
       </c>
       <c r="AE3">
-        <v>3.2924477350000001</v>
+        <v>3.5897974680769233</v>
       </c>
       <c r="AF3" t="s">
         <v>31</v>
@@ -9770,10 +9766,10 @@
         <v>31</v>
       </c>
       <c r="AH3">
-        <v>-23.579953140000001</v>
+        <v>-23.615299784615388</v>
       </c>
       <c r="AI3">
-        <v>13.2516865</v>
+        <v>12.931454542307693</v>
       </c>
       <c r="AJ3" s="7">
         <v>8.51</v>
@@ -10027,16 +10023,16 @@
         <v>3670.9015726696243</v>
       </c>
       <c r="AB4">
-        <v>50.442654920000003</v>
+        <v>48.130241346153859</v>
       </c>
       <c r="AC4">
-        <v>13.864247049999999</v>
+        <v>13.736281153307694</v>
       </c>
       <c r="AD4" t="s">
         <v>31</v>
       </c>
       <c r="AE4">
-        <v>3.6383263170000002</v>
+        <v>3.5897974680769233</v>
       </c>
       <c r="AF4" t="s">
         <v>31</v>
@@ -10045,10 +10041,10 @@
         <v>31</v>
       </c>
       <c r="AH4">
-        <v>-24.82197815</v>
+        <v>-23.615299784615388</v>
       </c>
       <c r="AI4">
-        <v>13.55605458</v>
+        <v>12.931454542307693</v>
       </c>
       <c r="AJ4" s="7">
         <v>8.51</v>
@@ -10302,16 +10298,16 @@
         <v>2432.2891785802917</v>
       </c>
       <c r="AB5">
-        <v>49.353448210000003</v>
+        <v>48.130241346153859</v>
       </c>
       <c r="AC5">
-        <v>14.41409494</v>
+        <v>13.736281153307694</v>
       </c>
       <c r="AD5" t="s">
         <v>31</v>
       </c>
       <c r="AE5">
-        <v>3.4239713570000001</v>
+        <v>3.5897974680769233</v>
       </c>
       <c r="AF5" t="s">
         <v>31</v>
@@ -10320,10 +10316,10 @@
         <v>31</v>
       </c>
       <c r="AH5">
-        <v>-24.048745220000001</v>
+        <v>-23.615299784615388</v>
       </c>
       <c r="AI5">
-        <v>12.74130587</v>
+        <v>12.931454542307693</v>
       </c>
       <c r="AJ5" s="7">
         <v>8.51</v>
@@ -10577,16 +10573,16 @@
         <v>2235.0599670628344</v>
       </c>
       <c r="AB6">
-        <v>45.834344119999997</v>
+        <v>48.130241346153859</v>
       </c>
       <c r="AC6">
-        <v>13.68383482</v>
+        <v>13.736281153307694</v>
       </c>
       <c r="AD6" t="s">
         <v>31</v>
       </c>
       <c r="AE6">
-        <v>3.3495248009999998</v>
+        <v>3.5897974680769233</v>
       </c>
       <c r="AF6" t="s">
         <v>31</v>
@@ -10595,10 +10591,10 @@
         <v>31</v>
       </c>
       <c r="AH6">
-        <v>-23.99557239</v>
+        <v>-23.615299784615388</v>
       </c>
       <c r="AI6">
-        <v>12.90011838</v>
+        <v>12.931454542307693</v>
       </c>
       <c r="AJ6" s="7">
         <v>8.51</v>
@@ -10852,16 +10848,16 @@
         <v>1656.2443511485969</v>
       </c>
       <c r="AB7">
-        <v>45.891883290000003</v>
+        <v>48.130241346153859</v>
       </c>
       <c r="AC7">
-        <v>14.02760546</v>
+        <v>13.736281153307694</v>
       </c>
       <c r="AD7" t="s">
         <v>31</v>
       </c>
       <c r="AE7">
-        <v>3.2715407779999999</v>
+        <v>3.5897974680769233</v>
       </c>
       <c r="AF7" t="s">
         <v>31</v>
@@ -10870,10 +10866,10 @@
         <v>31</v>
       </c>
       <c r="AH7">
-        <v>-23.983607960000001</v>
+        <v>-23.615299784615388</v>
       </c>
       <c r="AI7">
-        <v>12.33139493</v>
+        <v>12.931454542307693</v>
       </c>
       <c r="AJ7" s="7">
         <v>8.51</v>
@@ -15796,14 +15792,29 @@
         <f t="shared" si="8"/>
         <v>3441.6772221077067</v>
       </c>
+      <c r="AB26">
+        <v>48.130241346153859</v>
+      </c>
+      <c r="AC26">
+        <v>13.736281153307694</v>
+      </c>
       <c r="AD26" t="s">
         <v>31</v>
       </c>
+      <c r="AE26">
+        <v>3.5897974680769233</v>
+      </c>
       <c r="AF26" t="s">
         <v>31</v>
       </c>
       <c r="AG26" t="s">
         <v>31</v>
+      </c>
+      <c r="AH26">
+        <v>-23.615299784615388</v>
+      </c>
+      <c r="AI26">
+        <v>12.931454542307693</v>
       </c>
       <c r="AJ26" s="7">
         <v>8.49</v>
@@ -17138,16 +17149,16 @@
         <v>2842.1206317251458</v>
       </c>
       <c r="AB31">
-        <v>46.820824039999998</v>
+        <v>44.849519902307684</v>
       </c>
       <c r="AC31">
-        <v>14.28768788</v>
+        <v>13.606231183461539</v>
       </c>
       <c r="AD31" t="s">
         <v>31</v>
       </c>
       <c r="AE31">
-        <v>3.2770049609999998</v>
+        <v>3.2911418164615389</v>
       </c>
       <c r="AF31" t="s">
         <v>31</v>
@@ -17156,10 +17167,10 @@
         <v>31</v>
       </c>
       <c r="AH31">
-        <v>-23.886097759999998</v>
+        <v>-22.957768973076927</v>
       </c>
       <c r="AI31">
-        <v>12.58401098</v>
+        <v>13.280494286923076</v>
       </c>
       <c r="AJ31" s="7">
         <v>8.49</v>
@@ -17667,14 +17678,29 @@
         <f t="shared" si="8"/>
         <v>3071.1757577511162</v>
       </c>
+      <c r="AB33">
+        <v>48.130241346153859</v>
+      </c>
+      <c r="AC33">
+        <v>13.736281153307694</v>
+      </c>
       <c r="AD33" t="s">
         <v>31</v>
       </c>
+      <c r="AE33">
+        <v>3.5897974680769233</v>
+      </c>
       <c r="AF33" t="s">
         <v>31</v>
       </c>
       <c r="AG33" t="s">
         <v>31</v>
+      </c>
+      <c r="AH33">
+        <v>-23.615299784615388</v>
+      </c>
+      <c r="AI33">
+        <v>12.931454542307693</v>
       </c>
       <c r="AJ33">
         <v>8.4700000000000006</v>
@@ -17927,14 +17953,29 @@
         <f t="shared" si="8"/>
         <v>2371.244266987349</v>
       </c>
+      <c r="AB34">
+        <v>48.130241346153859</v>
+      </c>
+      <c r="AC34">
+        <v>13.736281153307694</v>
+      </c>
       <c r="AD34" t="s">
         <v>31</v>
       </c>
+      <c r="AE34">
+        <v>3.5897974680769233</v>
+      </c>
       <c r="AF34" t="s">
         <v>31</v>
       </c>
       <c r="AG34" t="s">
         <v>31</v>
+      </c>
+      <c r="AH34">
+        <v>-23.615299784615388</v>
+      </c>
+      <c r="AI34">
+        <v>12.931454542307693</v>
       </c>
       <c r="AJ34">
         <v>8.4700000000000006</v>
@@ -18188,16 +18229,16 @@
         <v>15275.106764049448</v>
       </c>
       <c r="AB35">
-        <v>44.942498649999997</v>
+        <v>51.794115875333326</v>
       </c>
       <c r="AC35">
-        <v>14.150903189999999</v>
+        <v>11.136419494933332</v>
       </c>
       <c r="AD35" t="s">
         <v>31</v>
       </c>
       <c r="AE35">
-        <v>3.175945595</v>
+        <v>5.0821599532666664</v>
       </c>
       <c r="AF35" t="s">
         <v>31</v>
@@ -18206,10 +18247,10 @@
         <v>31</v>
       </c>
       <c r="AH35">
-        <v>-23.480379859999999</v>
+        <v>-24.145373220666663</v>
       </c>
       <c r="AI35">
-        <v>11.50440961</v>
+        <v>11.343827143333334</v>
       </c>
       <c r="AJ35">
         <v>8.4700000000000006</v>
@@ -18463,16 +18504,16 @@
         <v>19399.629493172204</v>
       </c>
       <c r="AB36">
-        <v>43.323799899999997</v>
+        <v>51.794115875333326</v>
       </c>
       <c r="AC36">
-        <v>12.7768157</v>
+        <v>11.136419494933332</v>
       </c>
       <c r="AD36" t="s">
         <v>31</v>
       </c>
       <c r="AE36">
-        <v>3.390813557</v>
+        <v>5.0821599532666664</v>
       </c>
       <c r="AF36" t="s">
         <v>31</v>
@@ -18481,10 +18522,10 @@
         <v>31</v>
       </c>
       <c r="AH36">
-        <v>-24.30874549</v>
+        <v>-24.145373220666663</v>
       </c>
       <c r="AI36">
-        <v>10.85945626</v>
+        <v>11.343827143333334</v>
       </c>
       <c r="AJ36">
         <v>8.4700000000000006</v>
@@ -18738,16 +18779,16 @@
         <v>9190.1849384170073</v>
       </c>
       <c r="AB37">
-        <v>44.376729159999996</v>
+        <v>51.794115875333326</v>
       </c>
       <c r="AC37">
-        <v>14.06385596</v>
+        <v>11.136419494933332</v>
       </c>
       <c r="AD37" t="s">
         <v>31</v>
       </c>
       <c r="AE37">
-        <v>3.1553742640000002</v>
+        <v>5.0821599532666664</v>
       </c>
       <c r="AF37" t="s">
         <v>31</v>
@@ -18756,10 +18797,10 @@
         <v>31</v>
       </c>
       <c r="AH37">
-        <v>-23.583802439999999</v>
+        <v>-24.145373220666663</v>
       </c>
       <c r="AI37">
-        <v>12.325439190000001</v>
+        <v>11.343827143333334</v>
       </c>
       <c r="AJ37">
         <v>8.4700000000000006</v>
@@ -19273,16 +19314,16 @@
         <v>2698.909275762624</v>
       </c>
       <c r="AB39">
-        <v>46.958182299999997</v>
+        <v>48.130241346153859</v>
       </c>
       <c r="AC39">
-        <v>14.26518907</v>
+        <v>13.736281153307694</v>
       </c>
       <c r="AD39" t="s">
         <v>31</v>
       </c>
       <c r="AE39">
-        <v>3.2918023079999998</v>
+        <v>3.5897974680769233</v>
       </c>
       <c r="AF39" t="s">
         <v>31</v>
@@ -19291,10 +19332,10 @@
         <v>31</v>
       </c>
       <c r="AH39">
-        <v>-23.199938060000001</v>
+        <v>-23.615299784615388</v>
       </c>
       <c r="AI39">
-        <v>13.32790164</v>
+        <v>12.931454542307693</v>
       </c>
       <c r="AJ39">
         <v>8.4700000000000006</v>
@@ -19548,16 +19589,16 @@
         <v>3119.5225225396653</v>
       </c>
       <c r="AB40">
-        <v>47.341653639999997</v>
+        <v>48.130241346153859</v>
       </c>
       <c r="AC40">
-        <v>13.628827510000001</v>
+        <v>13.736281153307694</v>
       </c>
       <c r="AD40" t="s">
         <v>31</v>
       </c>
       <c r="AE40">
-        <v>3.4736409730000002</v>
+        <v>3.5897974680769233</v>
       </c>
       <c r="AF40" t="s">
         <v>31</v>
@@ -19566,10 +19607,10 @@
         <v>31</v>
       </c>
       <c r="AH40">
-        <v>-23.750301650000001</v>
+        <v>-23.615299784615388</v>
       </c>
       <c r="AI40">
-        <v>12.46836497</v>
+        <v>12.931454542307693</v>
       </c>
       <c r="AJ40">
         <v>8.4700000000000006</v>

</xml_diff>